<commit_message>
Changed rate values to be consistent with user defined time step
</commit_message>
<xml_diff>
--- a/GC_HIV_ModelParameters.xlsx
+++ b/GC_HIV_ModelParameters.xlsx
@@ -1185,8 +1185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:N117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1703,7 +1703,7 @@
         <v>118</v>
       </c>
       <c r="B49">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
@@ -1711,7 +1711,7 @@
         <v>144</v>
       </c>
       <c r="B50">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
@@ -1719,7 +1719,7 @@
         <v>119</v>
       </c>
       <c r="B51">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
@@ -1756,7 +1756,7 @@
         <v>123</v>
       </c>
       <c r="B57">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
@@ -1764,7 +1764,7 @@
         <v>124</v>
       </c>
       <c r="B58">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
@@ -1772,7 +1772,7 @@
         <v>145</v>
       </c>
       <c r="B59">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
@@ -1780,7 +1780,7 @@
         <v>146</v>
       </c>
       <c r="B60">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
@@ -1788,7 +1788,7 @@
         <v>119</v>
       </c>
       <c r="B61">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
@@ -1796,7 +1796,7 @@
         <v>125</v>
       </c>
       <c r="B62">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
@@ -1825,7 +1825,7 @@
         <v>132</v>
       </c>
       <c r="B67">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
@@ -1833,7 +1833,7 @@
         <v>133</v>
       </c>
       <c r="B68">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
@@ -1841,7 +1841,7 @@
         <v>134</v>
       </c>
       <c r="B69">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
@@ -1849,7 +1849,7 @@
         <v>135</v>
       </c>
       <c r="B70">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
@@ -1878,7 +1878,7 @@
         <v>139</v>
       </c>
       <c r="B75">
-        <v>0.15</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
@@ -1886,7 +1886,7 @@
         <v>140</v>
       </c>
       <c r="B76">
-        <v>0.15</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
@@ -1894,7 +1894,7 @@
         <v>141</v>
       </c>
       <c r="B77">
-        <v>0.15</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
@@ -1902,7 +1902,7 @@
         <v>142</v>
       </c>
       <c r="B78">
-        <v>0.15</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Adding notes about transition rates in spreadsheet
</commit_message>
<xml_diff>
--- a/GC_HIV_ModelParameters.xlsx
+++ b/GC_HIV_ModelParameters.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6760" tabRatio="682" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6760" tabRatio="682" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Model Parameters - Total" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="154">
   <si>
     <t>Symbol</t>
   </si>
@@ -473,6 +473,27 @@
   </si>
   <si>
     <t>kTreat_u_ps</t>
+  </si>
+  <si>
+    <t>Assume 90% present to care within 12 months of testing positive</t>
+  </si>
+  <si>
+    <t>Dropout rate = 0</t>
+  </si>
+  <si>
+    <t>routine testing every 6 months for HIV-positive</t>
+  </si>
+  <si>
+    <t>Rate of diagnosis = PS rate</t>
+  </si>
+  <si>
+    <t>No PS, no routine testing -&gt; diagnosis rate = 3 years</t>
+  </si>
+  <si>
+    <t>90% Test -&gt; Treat: 12 months</t>
+  </si>
+  <si>
+    <t>50% of infectious screen every 6 months</t>
   </si>
 </sst>
 </file>
@@ -1185,8 +1206,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:N117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B79" sqref="B79"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1687,7 +1708,7 @@
         <v>116</v>
       </c>
       <c r="B47">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
@@ -1695,10 +1716,10 @@
         <v>117</v>
       </c>
       <c r="B48">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>118</v>
       </c>
@@ -1706,7 +1727,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>144</v>
       </c>
@@ -1714,7 +1735,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>119</v>
       </c>
@@ -1722,7 +1743,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>120</v>
       </c>
@@ -1730,76 +1751,97 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" s="47" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>121</v>
       </c>
       <c r="B55">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>122</v>
       </c>
       <c r="B56">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+      <c r="F56" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>123</v>
       </c>
       <c r="B57">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="F57" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>124</v>
       </c>
       <c r="B58">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="F58" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>145</v>
       </c>
       <c r="B59">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="F59" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>146</v>
       </c>
       <c r="B60">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="F60" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>119</v>
       </c>
       <c r="B61">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="F61" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>125</v>
       </c>
       <c r="B62">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="F62" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" s="47" t="s">
         <v>129</v>
       </c>
@@ -1809,7 +1851,7 @@
         <v>130</v>
       </c>
       <c r="B65">
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
@@ -1817,7 +1859,7 @@
         <v>131</v>
       </c>
       <c r="B66">
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
@@ -1862,7 +1904,7 @@
         <v>137</v>
       </c>
       <c r="B73">
-        <v>0.15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
@@ -1870,7 +1912,7 @@
         <v>138</v>
       </c>
       <c r="B74">
-        <v>0.15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
@@ -2293,7 +2335,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
       <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Moved cells around to match up with loadUp script
</commit_message>
<xml_diff>
--- a/GC_HIV_ModelParameters.xlsx
+++ b/GC_HIV_ModelParameters.xlsx
@@ -5,22 +5,23 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicktzr\Google Drive\ICRC\AAPPS\Model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\AAPPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6760" tabRatio="682" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" tabRatio="682" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Model Parameters - Total" sheetId="1" r:id="rId1"/>
-    <sheet name="Rates" sheetId="8" r:id="rId2"/>
-    <sheet name="Partners" sheetId="9" r:id="rId3"/>
-    <sheet name="Model Parameters - HIV_N" sheetId="2" r:id="rId4"/>
-    <sheet name="Model Parameters - HIV_I" sheetId="3" r:id="rId5"/>
-    <sheet name="Model Parameters - HIV_K+V" sheetId="4" r:id="rId6"/>
-    <sheet name="Model Parameters - HIV_K" sheetId="6" r:id="rId7"/>
-    <sheet name="Model Parameters - HIV_V" sheetId="5" r:id="rId8"/>
-    <sheet name="HIV numbers by year" sheetId="7" r:id="rId9"/>
+    <sheet name="Rates" sheetId="11" r:id="rId2"/>
+    <sheet name="Targets" sheetId="10" r:id="rId3"/>
+    <sheet name="Partners" sheetId="9" r:id="rId4"/>
+    <sheet name="Model Parameters - HIV_N" sheetId="2" r:id="rId5"/>
+    <sheet name="Model Parameters - HIV_I" sheetId="3" r:id="rId6"/>
+    <sheet name="Model Parameters - HIV_K+V" sheetId="4" r:id="rId7"/>
+    <sheet name="Model Parameters - HIV_K" sheetId="6" r:id="rId8"/>
+    <sheet name="Model Parameters - HIV_V" sheetId="5" r:id="rId9"/>
+    <sheet name="HIV numbers by year" sheetId="7" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="159">
   <si>
     <t>Symbol</t>
   </si>
@@ -241,21 +242,6 @@
     <t>phaInt</t>
   </si>
   <si>
-    <t>HIV_N</t>
-  </si>
-  <si>
-    <t>HIV_I</t>
-  </si>
-  <si>
-    <t>HIV_K+V</t>
-  </si>
-  <si>
-    <t>HIV_K</t>
-  </si>
-  <si>
-    <t>HIV_V</t>
-  </si>
-  <si>
     <t>HIV Transmission</t>
   </si>
   <si>
@@ -337,48 +323,9 @@
     <t>(Same as HIV-V)</t>
   </si>
   <si>
-    <t>rec_r</t>
-  </si>
-  <si>
-    <t>ps_r</t>
-  </si>
-  <si>
-    <t>rec_u</t>
-  </si>
-  <si>
-    <t>rec_p</t>
-  </si>
-  <si>
-    <t>ps_u</t>
-  </si>
-  <si>
-    <t>ps_p</t>
-  </si>
-  <si>
     <t>P</t>
   </si>
   <si>
-    <t>r</t>
-  </si>
-  <si>
-    <t>u</t>
-  </si>
-  <si>
-    <t>p</t>
-  </si>
-  <si>
-    <t>Treated</t>
-  </si>
-  <si>
-    <t>Symptomatic</t>
-  </si>
-  <si>
-    <t>Partner Services</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>HIV parameters</t>
   </si>
   <si>
@@ -409,9 +356,6 @@
     <t>kTest_u_ps</t>
   </si>
   <si>
-    <t>kTreat_k_ps</t>
-  </si>
-  <si>
     <t>rTreat_v</t>
   </si>
   <si>
@@ -497,13 +441,85 @@
   </si>
   <si>
     <t>Natural Clearance Rates</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>Site proportions of those diagnosed with infection</t>
+  </si>
+  <si>
+    <t>Estimated proportion of GC-Infected that are screened and diagnosed</t>
+  </si>
+  <si>
+    <t>Test to treat rate</t>
+  </si>
+  <si>
+    <t>Proportion of diagnosed that are diagnosed by routine exam</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>prop_trt_r</t>
+  </si>
+  <si>
+    <t>prop_trt_u</t>
+  </si>
+  <si>
+    <t>prop_trt_p</t>
+  </si>
+  <si>
+    <t>Calculated in model script</t>
+  </si>
+  <si>
+    <t>Proportion of diagnosed that are diagnosed due to symptoms</t>
+  </si>
+  <si>
+    <t>prop_syptms_r</t>
+  </si>
+  <si>
+    <t>prop_syptms_u</t>
+  </si>
+  <si>
+    <t>prop_syptms_p</t>
+  </si>
+  <si>
+    <t>Proportion of diagnosed that are diagnosed by partner services</t>
+  </si>
+  <si>
+    <t>prop_PS_r</t>
+  </si>
+  <si>
+    <t>prop_PS_u</t>
+  </si>
+  <si>
+    <t>prop_PS_p</t>
+  </si>
+  <si>
+    <t>From test to treat rate</t>
+  </si>
+  <si>
+    <t>proportion of rectal diagnosed due to symptoms</t>
+  </si>
+  <si>
+    <t>proportion of urethral diagnosed due to symptoms</t>
+  </si>
+  <si>
+    <t>proportion of pharyngeal diagnosed due to symptoms</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -577,6 +593,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="19">
@@ -698,7 +720,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="14">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -713,8 +735,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -758,13 +781,12 @@
     <xf numFmtId="9" fontId="0" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="17" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="14">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -779,6 +801,7 @@
     <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent 2" xfId="14"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -1062,10 +1085,11 @@
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="64.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.08203125" customWidth="1"/>
+    <col min="3" max="3" width="65.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -1198,6 +1222,59 @@
       </c>
       <c r="D12" s="2" t="s">
         <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0.44</v>
       </c>
     </row>
   </sheetData>
@@ -1207,1139 +1284,1112 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:N117"/>
+  <dimension ref="A3:K93"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B3" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="44" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B5" s="45">
+        <v>0.65</v>
+      </c>
+      <c r="C5" s="45">
+        <v>0.65</v>
+      </c>
+      <c r="D5" s="45">
+        <v>0.65</v>
+      </c>
+      <c r="E5" s="45">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B6" s="45">
+        <v>0.91</v>
+      </c>
+      <c r="C6" s="45">
+        <v>0.91</v>
+      </c>
+      <c r="D6" s="45">
+        <v>0.91</v>
+      </c>
+      <c r="E6" s="45">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" s="45">
+        <v>0.75</v>
+      </c>
+      <c r="C7" s="45">
+        <v>0.75</v>
+      </c>
+      <c r="D7" s="45">
+        <v>0.75</v>
+      </c>
+      <c r="E7" s="45">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>143</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0.46</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.38</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0.35</v>
+      </c>
+      <c r="E11" s="5">
+        <v>0.43</v>
+      </c>
+      <c r="G11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>144</v>
+      </c>
+      <c r="B12" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.33</v>
+      </c>
+      <c r="D12" s="5">
+        <v>0.03</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0.09</v>
+      </c>
+      <c r="G12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>145</v>
+      </c>
+      <c r="B13" s="3">
+        <v>0.64</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.67</v>
+      </c>
+      <c r="D13" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="G13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>148</v>
+      </c>
+      <c r="B17" s="3">
+        <v>0.31</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.38</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.39</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0.32</v>
+      </c>
+      <c r="G17" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>149</v>
+      </c>
+      <c r="B18" s="3">
+        <v>0.88</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0.82</v>
+      </c>
+      <c r="G18" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>150</v>
+      </c>
+      <c r="B19" s="3">
+        <v>0.16</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0.19</v>
+      </c>
+      <c r="G19" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>152</v>
+      </c>
+      <c r="B23" s="3">
+        <v>0.22</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0.23</v>
+      </c>
+      <c r="D23" s="5">
+        <v>0.26</v>
+      </c>
+      <c r="E23" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="G23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>153</v>
+      </c>
+      <c r="B24" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0</v>
+      </c>
+      <c r="D24" s="5">
+        <v>0.09</v>
+      </c>
+      <c r="E24" s="5">
+        <v>0.09</v>
+      </c>
+      <c r="G24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>154</v>
+      </c>
+      <c r="B25" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0</v>
+      </c>
+      <c r="D25" s="5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E25" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="G25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28">
+        <v>0.9</v>
+      </c>
+      <c r="C28">
+        <v>0.9</v>
+      </c>
+      <c r="D28">
+        <v>0.9</v>
+      </c>
+      <c r="E28">
+        <v>0.9</v>
+      </c>
+      <c r="F28">
+        <v>0.9</v>
+      </c>
+      <c r="H28" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29">
+        <v>0.9</v>
+      </c>
+      <c r="C29">
+        <v>0.9</v>
+      </c>
+      <c r="D29">
+        <v>0.9</v>
+      </c>
+      <c r="E29">
+        <v>0.9</v>
+      </c>
+      <c r="F29">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30">
+        <v>0.9</v>
+      </c>
+      <c r="C30">
+        <v>0.9</v>
+      </c>
+      <c r="D30">
+        <v>0.9</v>
+      </c>
+      <c r="E30">
+        <v>0.9</v>
+      </c>
+      <c r="F30">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>67</v>
+      </c>
+      <c r="B33">
+        <f t="shared" ref="B33:F35" si="0">1/(185/365)</f>
+        <v>1.9729729729729728</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>1.9729729729729728</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>1.9729729729729728</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>1.9729729729729728</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="0"/>
+        <v>1.9729729729729728</v>
+      </c>
+      <c r="G33" s="3"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>68</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="0"/>
+        <v>1.9729729729729728</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>1.9729729729729728</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="0"/>
+        <v>1.9729729729729728</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>1.9729729729729728</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="0"/>
+        <v>1.9729729729729728</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>66</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="0"/>
+        <v>1.9729729729729728</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>1.9729729729729728</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="0"/>
+        <v>1.9729729729729728</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>1.9729729729729728</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="0"/>
+        <v>1.9729729729729728</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>52</v>
+      </c>
+      <c r="B37" s="46">
+        <f>1%</f>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>53</v>
+      </c>
+      <c r="B38" s="46">
+        <v>0.01</v>
+      </c>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B52" t="s">
         <v>69</v>
       </c>
-      <c r="C3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E3" t="s">
-        <v>72</v>
-      </c>
-      <c r="F3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B4" s="43">
-        <f t="array" ref="B4:B6">'Model Parameters - HIV_N'!C4:C6</f>
-        <v>0.37</v>
-      </c>
-      <c r="C4" s="44">
-        <f t="array" ref="C4:C6">'Model Parameters - HIV_I'!C25:C27</f>
-        <v>0.67</v>
-      </c>
-      <c r="D4" s="45">
-        <f t="array" ref="D4:D6">'Model Parameters - HIV_K+V'!C4:C6</f>
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="E4" s="3">
-        <f t="array" ref="E4:E6">'Model Parameters - HIV_K'!C4:C6</f>
-        <v>0.53</v>
-      </c>
-      <c r="F4" s="3">
-        <f t="array" ref="F4:F6">'Model Parameters - HIV_V'!C4:C6</f>
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B5" s="43">
-        <v>0.31</v>
-      </c>
-      <c r="C5" s="44">
-        <v>0.21</v>
-      </c>
-      <c r="D5" s="45">
-        <v>0.22</v>
-      </c>
-      <c r="E5" s="3">
-        <v>0.33</v>
-      </c>
-      <c r="F5" s="3">
-        <v>0.21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B6" s="43">
-        <v>0.32</v>
-      </c>
-      <c r="C6" s="44">
-        <v>0.12</v>
-      </c>
-      <c r="D6" s="45">
-        <v>0.22</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="F6" s="3">
-        <v>0.23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="I8" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>58</v>
-      </c>
-      <c r="B9">
-        <f t="shared" ref="B9:F10" si="0">1/(90/365)</f>
-        <v>4.0555555555555554</v>
-      </c>
-      <c r="C9">
-        <f t="shared" si="0"/>
-        <v>4.0555555555555554</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>4.0555555555555554</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="0"/>
-        <v>4.0555555555555554</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="0"/>
-        <v>4.0555555555555554</v>
-      </c>
-      <c r="J9">
-        <f>1/(145/365)</f>
-        <v>2.5172413793103448</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10">
-        <f t="shared" si="0"/>
-        <v>4.0555555555555554</v>
-      </c>
-      <c r="C10">
-        <f t="shared" si="0"/>
-        <v>4.0555555555555554</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="0"/>
-        <v>4.0555555555555554</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="0"/>
-        <v>4.0555555555555554</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="0"/>
-        <v>4.0555555555555554</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>57</v>
-      </c>
-      <c r="B11">
-        <f>1/(90/365)</f>
-        <v>4.0555555555555554</v>
-      </c>
-      <c r="C11">
-        <f>1/(90/365)</f>
-        <v>4.0555555555555554</v>
-      </c>
-      <c r="D11">
-        <f>1/(90/365)</f>
-        <v>4.0555555555555554</v>
-      </c>
-      <c r="E11">
-        <f>1/(90/365)</f>
-        <v>4.0555555555555554</v>
-      </c>
-      <c r="F11">
-        <f>1/(90/365)</f>
-        <v>4.0555555555555554</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>61</v>
-      </c>
-      <c r="B14">
-        <f t="shared" ref="B14:F15" si="1">1/(24/365)</f>
-        <v>15.208333333333336</v>
-      </c>
-      <c r="C14">
-        <f t="shared" si="1"/>
-        <v>15.208333333333336</v>
-      </c>
-      <c r="D14">
-        <f t="shared" si="1"/>
-        <v>15.208333333333336</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="1"/>
-        <v>15.208333333333336</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="1"/>
-        <v>15.208333333333336</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>62</v>
-      </c>
-      <c r="B15">
-        <f t="shared" si="1"/>
-        <v>15.208333333333336</v>
-      </c>
-      <c r="C15">
-        <f t="shared" si="1"/>
-        <v>15.208333333333336</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="1"/>
-        <v>15.208333333333336</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="1"/>
-        <v>15.208333333333336</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="1"/>
-        <v>15.208333333333336</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>60</v>
-      </c>
-      <c r="B16">
-        <f>1/(24/365)</f>
-        <v>15.208333333333336</v>
-      </c>
-      <c r="C16">
-        <f>1/(24/365)</f>
-        <v>15.208333333333336</v>
-      </c>
-      <c r="D16">
-        <f>1/(24/365)</f>
-        <v>15.208333333333336</v>
-      </c>
-      <c r="E16">
-        <f>1/(24/365)</f>
-        <v>15.208333333333336</v>
-      </c>
-      <c r="F16">
-        <f>1/(24/365)</f>
-        <v>15.208333333333336</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>64</v>
-      </c>
-      <c r="B19">
-        <f t="shared" ref="B19:F20" si="2">1/(12/365)</f>
-        <v>30.416666666666671</v>
-      </c>
-      <c r="C19">
-        <f t="shared" si="2"/>
-        <v>30.416666666666671</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="2"/>
-        <v>30.416666666666671</v>
-      </c>
-      <c r="E19">
-        <f t="shared" si="2"/>
-        <v>30.416666666666671</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="2"/>
-        <v>30.416666666666671</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>65</v>
-      </c>
-      <c r="B20">
-        <f t="shared" si="2"/>
-        <v>30.416666666666671</v>
-      </c>
-      <c r="C20">
-        <f t="shared" si="2"/>
-        <v>30.416666666666671</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="2"/>
-        <v>30.416666666666671</v>
-      </c>
-      <c r="E20">
-        <f t="shared" si="2"/>
-        <v>30.416666666666671</v>
-      </c>
-      <c r="F20">
-        <f t="shared" si="2"/>
-        <v>30.416666666666671</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>63</v>
-      </c>
-      <c r="B21">
-        <f>1/(12/365)</f>
-        <v>30.416666666666671</v>
-      </c>
-      <c r="C21">
-        <f>1/(12/365)</f>
-        <v>30.416666666666671</v>
-      </c>
-      <c r="D21">
-        <f>1/(12/365)</f>
-        <v>30.416666666666671</v>
-      </c>
-      <c r="E21">
-        <f>1/(12/365)</f>
-        <v>30.416666666666671</v>
-      </c>
-      <c r="F21">
-        <f>1/(12/365)</f>
-        <v>30.416666666666671</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>67</v>
-      </c>
-      <c r="B24">
-        <f>1/(185/365)</f>
-        <v>1.9729729729729728</v>
-      </c>
-      <c r="C24">
-        <f t="shared" ref="C24:F24" si="3">1/(185/365)</f>
-        <v>1.9729729729729728</v>
-      </c>
-      <c r="D24">
-        <f t="shared" si="3"/>
-        <v>1.9729729729729728</v>
-      </c>
-      <c r="E24">
-        <f t="shared" si="3"/>
-        <v>1.9729729729729728</v>
-      </c>
-      <c r="F24">
-        <f t="shared" si="3"/>
-        <v>1.9729729729729728</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>68</v>
-      </c>
-      <c r="B25">
-        <f t="shared" ref="B25:F26" si="4">1/(185/365)</f>
-        <v>1.9729729729729728</v>
-      </c>
-      <c r="C25">
-        <f t="shared" si="4"/>
-        <v>1.9729729729729728</v>
-      </c>
-      <c r="D25">
-        <f t="shared" si="4"/>
-        <v>1.9729729729729728</v>
-      </c>
-      <c r="E25">
-        <f t="shared" si="4"/>
-        <v>1.9729729729729728</v>
-      </c>
-      <c r="F25">
-        <f t="shared" si="4"/>
-        <v>1.9729729729729728</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>66</v>
-      </c>
-      <c r="B26">
-        <f t="shared" si="4"/>
-        <v>1.9729729729729728</v>
-      </c>
-      <c r="C26">
-        <f t="shared" si="4"/>
-        <v>1.9729729729729728</v>
-      </c>
-      <c r="D26">
-        <f t="shared" si="4"/>
-        <v>1.9729729729729728</v>
-      </c>
-      <c r="E26">
-        <f t="shared" si="4"/>
-        <v>1.9729729729729728</v>
-      </c>
-      <c r="F26">
-        <f t="shared" si="4"/>
-        <v>1.9729729729729728</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>52</v>
-      </c>
-      <c r="B29" s="13">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>53</v>
-      </c>
-      <c r="B30" s="13">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B35" t="s">
-        <v>74</v>
-      </c>
-      <c r="C35">
+      <c r="C52">
         <f>0.82*10^-2</f>
         <v>8.199999999999999E-3</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D52" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>80</v>
+      </c>
+      <c r="B53" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>85</v>
-      </c>
-      <c r="B36" t="s">
+      <c r="C53">
+        <v>0.84</v>
+      </c>
+      <c r="D53" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
         <v>80</v>
       </c>
-      <c r="C36">
-        <v>0.84</v>
-      </c>
-      <c r="D36" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>85</v>
-      </c>
-      <c r="B37" t="s">
-        <v>82</v>
-      </c>
-      <c r="C37">
+      <c r="B54" t="s">
+        <v>77</v>
+      </c>
+      <c r="C54">
         <v>0.24299999999999999</v>
       </c>
-      <c r="D37" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>85</v>
-      </c>
-      <c r="B38" t="s">
-        <v>83</v>
-      </c>
-      <c r="C38">
+      <c r="D54" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>80</v>
+      </c>
+      <c r="B55" t="s">
+        <v>78</v>
+      </c>
+      <c r="C55">
         <v>0.62</v>
       </c>
-      <c r="D38" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41" s="46" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A43" s="47" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>126</v>
-      </c>
-      <c r="B44">
+      <c r="D55" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K57" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A58" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="K58" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K59" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A60" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="K60" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>107</v>
+      </c>
+      <c r="B61">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A46" s="47" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>116</v>
-      </c>
-      <c r="B47">
+      <c r="K61" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K62" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A63" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="B63" t="s">
+        <v>41</v>
+      </c>
+      <c r="C63" t="s">
+        <v>42</v>
+      </c>
+      <c r="D63" t="s">
+        <v>43</v>
+      </c>
+      <c r="E63" t="s">
+        <v>44</v>
+      </c>
+      <c r="K63" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>98</v>
+      </c>
+      <c r="B64">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>117</v>
-      </c>
-      <c r="B48">
+      <c r="C64">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>118</v>
-      </c>
-      <c r="B49">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>144</v>
-      </c>
-      <c r="B50">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>119</v>
-      </c>
-      <c r="B51">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
-        <v>120</v>
-      </c>
-      <c r="B52">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A54" s="47" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
-        <v>121</v>
-      </c>
-      <c r="B55">
+      <c r="D64">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
-        <v>122</v>
-      </c>
-      <c r="B56">
+      <c r="E64">
         <v>0</v>
       </c>
-      <c r="F56" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
-        <v>123</v>
-      </c>
-      <c r="B57">
-        <v>0.4</v>
-      </c>
-      <c r="F57" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
-        <v>124</v>
-      </c>
-      <c r="B58">
-        <v>0.4</v>
-      </c>
-      <c r="F58" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
-        <v>145</v>
-      </c>
-      <c r="B59">
-        <v>0.4</v>
-      </c>
-      <c r="F59" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
-        <v>146</v>
-      </c>
-      <c r="B60">
-        <v>0.4</v>
-      </c>
-      <c r="F60" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
-        <v>119</v>
-      </c>
-      <c r="B61">
-        <v>0.4</v>
-      </c>
-      <c r="F61" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
-        <v>125</v>
-      </c>
-      <c r="B62">
-        <v>0.4</v>
-      </c>
-      <c r="F62" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A64" s="47" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>130</v>
+        <v>99</v>
       </c>
       <c r="B65">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>131</v>
-      </c>
-      <c r="B66">
+        <v>100</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>125</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>101</v>
+      </c>
+      <c r="B68">
+        <v>0.9</v>
+      </c>
+      <c r="C68">
+        <v>0.9</v>
+      </c>
+      <c r="D68">
+        <v>0.9</v>
+      </c>
+      <c r="E68">
+        <v>0.9</v>
+      </c>
+      <c r="G68" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>102</v>
+      </c>
+      <c r="B69">
+        <v>0.9</v>
+      </c>
+      <c r="C69">
+        <v>0.9</v>
+      </c>
+      <c r="D69">
+        <v>0.9</v>
+      </c>
+      <c r="E69">
+        <v>0.9</v>
+      </c>
+      <c r="G69" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A71" s="44" t="s">
+        <v>108</v>
+      </c>
+      <c r="B71" t="s">
+        <v>41</v>
+      </c>
+      <c r="C71" t="s">
+        <v>42</v>
+      </c>
+      <c r="D71" t="s">
+        <v>43</v>
+      </c>
+      <c r="E71" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>103</v>
+      </c>
+      <c r="B72">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A67" t="s">
-        <v>132</v>
-      </c>
-      <c r="B67">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A68" t="s">
-        <v>133</v>
-      </c>
-      <c r="B68">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A69" t="s">
-        <v>134</v>
-      </c>
-      <c r="B69">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A70" t="s">
-        <v>135</v>
-      </c>
-      <c r="B70">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A72" s="47" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>137</v>
+        <v>104</v>
       </c>
       <c r="B73">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C73">
+        <v>0</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>138</v>
-      </c>
-      <c r="B74">
+        <v>105</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>106</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>126</v>
+      </c>
+      <c r="B76">
+        <v>0.9</v>
+      </c>
+      <c r="C76">
+        <v>0.9</v>
+      </c>
+      <c r="D76">
+        <v>0.9</v>
+      </c>
+      <c r="E76">
+        <v>0.9</v>
+      </c>
+      <c r="G76" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>127</v>
+      </c>
+      <c r="B77">
+        <v>0.9</v>
+      </c>
+      <c r="C77">
+        <v>0.9</v>
+      </c>
+      <c r="D77">
+        <v>0.9</v>
+      </c>
+      <c r="E77">
+        <v>0.9</v>
+      </c>
+      <c r="G77" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A79" s="44" t="s">
+        <v>110</v>
+      </c>
+      <c r="B79" t="s">
+        <v>41</v>
+      </c>
+      <c r="C79" t="s">
+        <v>42</v>
+      </c>
+      <c r="D79" t="s">
+        <v>43</v>
+      </c>
+      <c r="E79" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>111</v>
+      </c>
+      <c r="B80">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A75" t="s">
-        <v>139</v>
-      </c>
-      <c r="B75">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A76" t="s">
-        <v>140</v>
-      </c>
-      <c r="B76">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A77" t="s">
-        <v>141</v>
-      </c>
-      <c r="B77">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A78" t="s">
-        <v>142</v>
-      </c>
-      <c r="B78">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="C80">
+        <v>0</v>
+      </c>
+      <c r="D80">
+        <v>0</v>
+      </c>
+      <c r="E80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>112</v>
+      </c>
+      <c r="B81">
+        <v>0</v>
+      </c>
+      <c r="C81">
+        <v>0</v>
+      </c>
+      <c r="D81">
+        <v>0</v>
+      </c>
+      <c r="E81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>113</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>114</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>115</v>
+      </c>
+      <c r="B84">
+        <v>0.9</v>
+      </c>
+      <c r="C84">
+        <v>0.9</v>
+      </c>
+      <c r="D84">
+        <v>0.9</v>
+      </c>
+      <c r="E84">
+        <v>0.9</v>
+      </c>
+      <c r="G84" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>116</v>
+      </c>
+      <c r="B85">
+        <v>0.9</v>
+      </c>
+      <c r="C85">
+        <v>0.9</v>
+      </c>
+      <c r="D85">
+        <v>0.9</v>
+      </c>
+      <c r="E85">
+        <v>0.9</v>
+      </c>
+      <c r="G85" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A87" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="B87" t="s">
+        <v>41</v>
+      </c>
+      <c r="C87" t="s">
+        <v>42</v>
+      </c>
+      <c r="D87" t="s">
+        <v>43</v>
+      </c>
+      <c r="E87" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+        <v>118</v>
+      </c>
+      <c r="B88">
+        <v>0</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
+      </c>
+      <c r="D88">
+        <v>0</v>
+      </c>
+      <c r="E88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+        <v>119</v>
+      </c>
+      <c r="B89">
+        <v>0</v>
+      </c>
+      <c r="C89">
+        <v>0</v>
+      </c>
+      <c r="D89">
+        <v>0</v>
+      </c>
+      <c r="E89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+        <v>120</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E90" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>121</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E91" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+        <v>122</v>
+      </c>
+      <c r="B92">
+        <v>0.9</v>
+      </c>
+      <c r="C92">
+        <v>0.9</v>
+      </c>
+      <c r="D92">
+        <v>0.9</v>
+      </c>
+      <c r="E92">
+        <v>0.9</v>
+      </c>
+      <c r="G92" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A94" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A96" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A97" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A98" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A101" t="s">
-        <v>111</v>
-      </c>
-      <c r="I101" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B102" t="s">
-        <v>41</v>
-      </c>
-      <c r="C102" t="s">
-        <v>42</v>
-      </c>
-      <c r="D102" t="s">
-        <v>43</v>
-      </c>
-      <c r="E102" t="s">
-        <v>44</v>
-      </c>
-      <c r="F102" t="s">
-        <v>107</v>
-      </c>
-      <c r="J102" t="s">
-        <v>41</v>
-      </c>
-      <c r="K102" t="s">
-        <v>42</v>
-      </c>
-      <c r="L102" t="s">
-        <v>43</v>
-      </c>
-      <c r="M102" t="s">
-        <v>44</v>
-      </c>
-      <c r="N102" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A103" t="s">
-        <v>108</v>
-      </c>
-      <c r="B103">
-        <v>0.46</v>
-      </c>
-      <c r="C103">
-        <v>0.38</v>
-      </c>
-      <c r="D103">
-        <v>0.35</v>
-      </c>
-      <c r="E103">
-        <v>0.43</v>
-      </c>
-      <c r="F103">
-        <v>0.51</v>
-      </c>
-      <c r="I103" t="s">
-        <v>108</v>
-      </c>
-      <c r="J103">
-        <f t="shared" ref="J103:N105" si="5">B103+B109+B115</f>
-        <v>1</v>
-      </c>
-      <c r="K103">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="L103">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="M103">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="N103">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A104" t="s">
-        <v>109</v>
-      </c>
-      <c r="B104">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C104">
-        <v>0.33</v>
-      </c>
-      <c r="D104">
-        <v>0.03</v>
-      </c>
-      <c r="E104">
-        <v>0.09</v>
-      </c>
-      <c r="F104">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="I104" t="s">
-        <v>109</v>
-      </c>
-      <c r="J104">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="K104">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="L104">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="M104">
-        <f t="shared" si="5"/>
-        <v>0.99999999999999989</v>
-      </c>
-      <c r="N104">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A105" t="s">
-        <v>110</v>
-      </c>
-      <c r="B105">
-        <v>0.64</v>
-      </c>
-      <c r="C105">
-        <v>0.67</v>
-      </c>
-      <c r="D105">
-        <v>0.6</v>
-      </c>
-      <c r="E105">
-        <v>0.6</v>
-      </c>
-      <c r="F105">
-        <v>0.69</v>
-      </c>
-      <c r="I105" t="s">
-        <v>110</v>
-      </c>
-      <c r="J105">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="K105">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="L105">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="M105">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="N105">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A107" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B108" t="s">
-        <v>41</v>
-      </c>
-      <c r="C108" t="s">
-        <v>42</v>
-      </c>
-      <c r="D108" t="s">
-        <v>43</v>
-      </c>
-      <c r="E108" t="s">
-        <v>44</v>
-      </c>
-      <c r="F108" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A109" t="s">
-        <v>108</v>
-      </c>
-      <c r="B109">
-        <v>0.31</v>
-      </c>
-      <c r="C109">
-        <v>0.39</v>
-      </c>
-      <c r="D109">
-        <v>0.39</v>
-      </c>
-      <c r="E109">
-        <v>0.32</v>
-      </c>
-      <c r="F109">
-        <v>0.16</v>
-      </c>
-    </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A110" t="s">
-        <v>109</v>
-      </c>
-      <c r="B110">
-        <v>0.88</v>
-      </c>
-      <c r="C110">
-        <v>0.67</v>
-      </c>
-      <c r="D110">
-        <v>0.88</v>
-      </c>
-      <c r="E110">
-        <v>0.82</v>
-      </c>
-      <c r="F110">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A111" t="s">
-        <v>110</v>
-      </c>
-      <c r="B111">
-        <v>0.16</v>
-      </c>
-      <c r="C111">
-        <v>0.33</v>
-      </c>
-      <c r="D111">
-        <v>0.33</v>
-      </c>
-      <c r="E111">
-        <v>0.2</v>
-      </c>
-      <c r="F111">
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A113" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B114" t="s">
-        <v>41</v>
-      </c>
-      <c r="C114" t="s">
-        <v>42</v>
-      </c>
-      <c r="D114" t="s">
-        <v>43</v>
-      </c>
-      <c r="E114" t="s">
-        <v>44</v>
-      </c>
-      <c r="F114" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A115" t="s">
-        <v>108</v>
-      </c>
-      <c r="B115">
-        <v>0.23</v>
-      </c>
-      <c r="C115">
-        <v>0.23</v>
-      </c>
-      <c r="D115">
-        <v>0.26</v>
-      </c>
-      <c r="E115">
-        <v>0.25</v>
-      </c>
-      <c r="F115">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A116" t="s">
-        <v>109</v>
-      </c>
-      <c r="B116">
-        <v>0.05</v>
-      </c>
-      <c r="C116">
-        <v>0</v>
-      </c>
-      <c r="D116">
-        <v>0.09</v>
-      </c>
-      <c r="E116">
-        <v>0.09</v>
-      </c>
-      <c r="F116">
-        <v>0.81</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A117" t="s">
-        <v>110</v>
-      </c>
-      <c r="B117">
-        <v>0.2</v>
-      </c>
-      <c r="C117">
-        <v>0</v>
-      </c>
-      <c r="D117">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="E117">
-        <v>0.2</v>
-      </c>
-      <c r="F117">
-        <v>0.2</v>
+        <v>123</v>
+      </c>
+      <c r="B93">
+        <v>0.9</v>
+      </c>
+      <c r="C93">
+        <v>0.9</v>
+      </c>
+      <c r="D93">
+        <v>0.9</v>
+      </c>
+      <c r="E93">
+        <v>0.9</v>
+      </c>
+      <c r="G93" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -2350,25 +2400,110 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B2" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="44" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="44" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="44" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="44" t="s">
+        <v>136</v>
+      </c>
+      <c r="B3" s="45">
+        <v>0.37</v>
+      </c>
+      <c r="C3" s="45">
+        <v>0.74</v>
+      </c>
+      <c r="D3" s="45">
+        <v>0.53</v>
+      </c>
+      <c r="E3" s="45">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="44" t="s">
+        <v>137</v>
+      </c>
+      <c r="B4" s="45">
+        <v>0.31</v>
+      </c>
+      <c r="C4" s="45">
+        <v>0.17</v>
+      </c>
+      <c r="D4" s="45">
+        <v>0.33</v>
+      </c>
+      <c r="E4" s="45">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="44" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" s="45">
+        <v>0.32</v>
+      </c>
+      <c r="C5" s="45">
+        <v>0.09</v>
+      </c>
+      <c r="D5" s="45">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E5" s="45">
+        <v>0.23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="46" t="s">
-        <v>86</v>
+      <c r="A1" s="43" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -2389,56 +2524,56 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B7" s="3">
         <v>0.65</v>
       </c>
       <c r="C7" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B8" s="3">
         <v>0.56000000000000005</v>
       </c>
       <c r="C8" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B9" s="3">
         <v>0.38</v>
       </c>
       <c r="C9" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="46" t="s">
-        <v>93</v>
+      <c r="A11" s="43" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B12" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -2459,61 +2594,61 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B17" s="3">
         <v>0.89</v>
       </c>
       <c r="C17" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B18" s="3">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B19" s="3">
         <v>0.67</v>
       </c>
       <c r="C19" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" s="46" t="s">
-        <v>94</v>
+      <c r="A22" s="43" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B23" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B24">
         <v>6</v>
@@ -2521,7 +2656,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -2529,65 +2664,65 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="B26">
-        <v>19</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B28" s="1">
         <v>0.78</v>
       </c>
       <c r="C28" t="s">
+        <v>85</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B29" s="1">
         <v>0.76</v>
       </c>
       <c r="C29" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B30" s="1">
         <v>0.49</v>
       </c>
       <c r="C30" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A33" s="46" t="s">
-        <v>98</v>
+      <c r="A33" s="43" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B34" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
@@ -2608,59 +2743,59 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B37">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B39">
         <v>0.78</v>
       </c>
       <c r="C39" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B40">
         <v>0.7</v>
       </c>
       <c r="C40" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B41">
         <v>0.69</v>
       </c>
       <c r="C41" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A44" s="46" t="s">
-        <v>99</v>
+      <c r="A44" s="43" t="s">
+        <v>94</v>
       </c>
       <c r="B44" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B45" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
@@ -2681,15 +2816,15 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B48">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B50">
         <v>0.78</v>
@@ -2697,7 +2832,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B51">
         <v>0.7</v>
@@ -2705,7 +2840,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B52">
         <v>0.69</v>
@@ -2717,7 +2852,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F39"/>
   <sheetViews>
@@ -2725,7 +2860,7 @@
       <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
@@ -3373,7 +3508,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G39"/>
   <sheetViews>
@@ -3381,7 +3516,7 @@
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.5" style="3" bestFit="1" customWidth="1"/>
@@ -4080,7 +4215,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F23"/>
   <sheetViews>
@@ -4088,7 +4223,7 @@
       <selection activeCell="C10" sqref="C10:C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.5" style="1" bestFit="1" customWidth="1"/>
@@ -4440,15 +4575,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B18"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.5" style="1" bestFit="1" customWidth="1"/>
@@ -4795,15 +4930,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4:B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.5" style="1" bestFit="1" customWidth="1"/>
@@ -5148,57 +5283,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>77</v>
-      </c>
-      <c r="B9" s="3">
-        <v>0.19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>78</v>
-      </c>
-      <c r="B10" s="3">
-        <v>0.44</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
added new MSM pop, observed HIV prevalence and incidence
</commit_message>
<xml_diff>
--- a/GC_HIV_ModelParameters.xlsx
+++ b/GC_HIV_ModelParameters.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\AAPS_model\AAPPS_7\AAPPS-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\AAPS_model\AAPPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700" tabRatio="682" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700" tabRatio="682" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="References" sheetId="12" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1003" uniqueCount="326">
   <si>
     <t>Symbol</t>
   </si>
@@ -923,16 +923,107 @@
   </si>
   <si>
     <t>Khurana, 2018 (https://bit.ly/2UV2Sj1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HIV prevalence </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Years </t>
+  </si>
+  <si>
+    <t>Prevalent HIV cases (KC HIV reports)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rectal GC cases </t>
+  </si>
+  <si>
+    <t>Urethral GC cases</t>
+  </si>
+  <si>
+    <t>Pharyngeal GC cases</t>
+  </si>
+  <si>
+    <t># New HIV dx (2017 HIV epi report)</t>
+  </si>
+  <si>
+    <t>new HIV dx rate (per 100,000), not including MSM who inject drugs</t>
+  </si>
+  <si>
+    <t>dx'ed HIV Prevalence (2017 KC HIV AIDS report)</t>
+  </si>
+  <si>
+    <t># MSM in KC</t>
+  </si>
+  <si>
+    <t>Male aged 15+ population (WA OFM data)</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>15-19</t>
+  </si>
+  <si>
+    <t>20-24</t>
+  </si>
+  <si>
+    <t>25-29</t>
+  </si>
+  <si>
+    <t>30-34</t>
+  </si>
+  <si>
+    <t>35-39</t>
+  </si>
+  <si>
+    <t>40-44</t>
+  </si>
+  <si>
+    <t>45-49</t>
+  </si>
+  <si>
+    <t>50-54</t>
+  </si>
+  <si>
+    <t>55-59</t>
+  </si>
+  <si>
+    <t>60-64</t>
+  </si>
+  <si>
+    <t>65-69</t>
+  </si>
+  <si>
+    <t>70-74</t>
+  </si>
+  <si>
+    <t>75-79</t>
+  </si>
+  <si>
+    <t>80-84</t>
+  </si>
+  <si>
+    <t>85+</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Black = HIV epi report</t>
+  </si>
+  <si>
+    <t>Red = calculated with new pop estimates</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="170" formatCode="0.0"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1066,6 +1157,12 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1507,7 +1604,7 @@
     <xf numFmtId="0" fontId="2" fillId="22" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="27" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1632,6 +1729,9 @@
     <xf numFmtId="0" fontId="15" fillId="23" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="20">
     <cellStyle name="Bad" xfId="16" builtinId="27"/>
@@ -1683,8 +1783,8 @@
       <xdr:rowOff>104776</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>169877</xdr:rowOff>
     </xdr:to>
@@ -1751,8 +1851,8 @@
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
       <xdr:row>65</xdr:row>
       <xdr:rowOff>104069</xdr:rowOff>
     </xdr:to>
@@ -3878,7 +3978,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:V94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
@@ -5473,18 +5573,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J97"/>
+  <dimension ref="A1:M131"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="A98" sqref="A98"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="D114" sqref="D114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.75" customWidth="1"/>
-    <col min="2" max="2" width="19.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="14.75" customWidth="1"/>
+    <col min="4" max="4" width="20.5" customWidth="1"/>
+    <col min="5" max="5" width="13.25" customWidth="1"/>
     <col min="6" max="6" width="12.625" customWidth="1"/>
     <col min="7" max="7" width="13.5" customWidth="1"/>
   </cols>
@@ -5921,7 +6022,7 @@
         <v>31.224489795918299</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>295</v>
       </c>
@@ -5936,6 +6037,996 @@
       </c>
       <c r="H97" t="s">
         <v>294</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>297</v>
+      </c>
+      <c r="B101" t="s">
+        <v>302</v>
+      </c>
+      <c r="C101" t="s">
+        <v>303</v>
+      </c>
+      <c r="D101" t="s">
+        <v>298</v>
+      </c>
+      <c r="E101" t="s">
+        <v>304</v>
+      </c>
+      <c r="F101" t="s">
+        <v>299</v>
+      </c>
+      <c r="G101" t="s">
+        <v>300</v>
+      </c>
+      <c r="H101" t="s">
+        <v>301</v>
+      </c>
+      <c r="I101" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>2008</v>
+      </c>
+      <c r="C102">
+        <v>506.7</v>
+      </c>
+      <c r="D102">
+        <f>4377+537</f>
+        <v>4914</v>
+      </c>
+      <c r="E102" s="93">
+        <f>D102/I102*100</f>
+        <v>11.183347708509524</v>
+      </c>
+      <c r="I102" s="10">
+        <f>0.057*C131</f>
+        <v>43940.330999999998</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>2009</v>
+      </c>
+      <c r="B103">
+        <v>223</v>
+      </c>
+      <c r="C103">
+        <v>517.20000000000005</v>
+      </c>
+      <c r="D103">
+        <f>4525+555</f>
+        <v>5080</v>
+      </c>
+      <c r="E103" s="93">
+        <f t="shared" ref="E103:E107" si="0">D103/I103*100</f>
+        <v>11.444414669441711</v>
+      </c>
+      <c r="I103" s="10">
+        <f>0.057*D131</f>
+        <v>44388.465000000004</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>2010</v>
+      </c>
+      <c r="B104">
+        <v>256</v>
+      </c>
+      <c r="C104">
+        <v>580.5</v>
+      </c>
+      <c r="D104">
+        <f>4668+562</f>
+        <v>5230</v>
+      </c>
+      <c r="E104" s="93">
+        <f t="shared" si="0"/>
+        <v>11.677404184944985</v>
+      </c>
+      <c r="I104" s="10">
+        <f>0.057*E131</f>
+        <v>44787.351000000002</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>2011</v>
+      </c>
+      <c r="B105">
+        <v>205</v>
+      </c>
+      <c r="C105">
+        <v>494.4</v>
+      </c>
+      <c r="D105">
+        <f>4792+592</f>
+        <v>5384</v>
+      </c>
+      <c r="E105" s="93">
+        <f t="shared" si="0"/>
+        <v>11.937626066106644</v>
+      </c>
+      <c r="I105" s="10">
+        <f>0.057*F131</f>
+        <v>45101.094389999991</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>2012</v>
+      </c>
+      <c r="B106">
+        <f>168+27</f>
+        <v>195</v>
+      </c>
+      <c r="C106">
+        <v>482.1</v>
+      </c>
+      <c r="D106">
+        <f>4904+612</f>
+        <v>5516</v>
+      </c>
+      <c r="E106" s="93">
+        <f t="shared" si="0"/>
+        <v>12.1282712404082</v>
+      </c>
+      <c r="I106" s="10">
+        <f>0.057*G131</f>
+        <v>45480.513179999994</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>2013</v>
+      </c>
+      <c r="B107">
+        <f>50+17</f>
+        <v>67</v>
+      </c>
+      <c r="C107">
+        <v>407.2</v>
+      </c>
+      <c r="D107">
+        <f>5145+683</f>
+        <v>5828</v>
+      </c>
+      <c r="E107" s="93">
+        <f t="shared" si="0"/>
+        <v>12.638456401528872</v>
+      </c>
+      <c r="I107" s="10">
+        <f>0.057*H131</f>
+        <v>46113.226289999999</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>2014</v>
+      </c>
+      <c r="B108">
+        <f>156+16</f>
+        <v>172</v>
+      </c>
+      <c r="C108">
+        <v>374</v>
+      </c>
+      <c r="D108">
+        <f>4664+611</f>
+        <v>5275</v>
+      </c>
+      <c r="E108" s="93">
+        <f>D108/I108*100</f>
+        <v>10.317495369778975</v>
+      </c>
+      <c r="I108" s="10">
+        <f>0.062*I131</f>
+        <v>51126.749379999994</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>2015</v>
+      </c>
+      <c r="B109">
+        <f>146+7</f>
+        <v>153</v>
+      </c>
+      <c r="C109">
+        <v>320.39999999999998</v>
+      </c>
+      <c r="D109">
+        <f>4745+596</f>
+        <v>5341</v>
+      </c>
+      <c r="E109" s="93">
+        <f>D109/I109*100</f>
+        <v>10.085576513264584</v>
+      </c>
+      <c r="I109" s="10">
+        <f>0.063*J131</f>
+        <v>52956.814050000008</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>2016</v>
+      </c>
+      <c r="B110">
+        <f>112+14</f>
+        <v>126</v>
+      </c>
+      <c r="C110">
+        <v>251.9</v>
+      </c>
+      <c r="D110">
+        <f>4598+601</f>
+        <v>5199</v>
+      </c>
+      <c r="E110" s="93">
+        <f>D110/I110*100</f>
+        <v>9.4106768370489764</v>
+      </c>
+      <c r="I110" s="10">
+        <f>0.064*K131</f>
+        <v>55245.760639999993</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>2017</v>
+      </c>
+      <c r="B111">
+        <f>103+10</f>
+        <v>113</v>
+      </c>
+      <c r="C111">
+        <v>220</v>
+      </c>
+      <c r="D111">
+        <v>5269</v>
+      </c>
+      <c r="E111">
+        <v>9.0299999999999994</v>
+      </c>
+      <c r="I111" s="10">
+        <f>0.066*L131</f>
+        <v>58353.280259999992</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A112" s="6" t="s">
+        <v>325</v>
+      </c>
+      <c r="E112" s="92"/>
+    </row>
+    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A113" s="94" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>307</v>
+      </c>
+      <c r="B115">
+        <v>2007</v>
+      </c>
+      <c r="C115">
+        <v>2008</v>
+      </c>
+      <c r="D115">
+        <v>2009</v>
+      </c>
+      <c r="E115">
+        <v>2010</v>
+      </c>
+      <c r="F115">
+        <v>2011</v>
+      </c>
+      <c r="G115">
+        <v>2012</v>
+      </c>
+      <c r="H115">
+        <v>2013</v>
+      </c>
+      <c r="I115">
+        <v>2014</v>
+      </c>
+      <c r="J115">
+        <v>2015</v>
+      </c>
+      <c r="K115">
+        <v>2016</v>
+      </c>
+      <c r="L115">
+        <v>2017</v>
+      </c>
+      <c r="M115">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>308</v>
+      </c>
+      <c r="B116">
+        <v>59783</v>
+      </c>
+      <c r="C116">
+        <v>60240</v>
+      </c>
+      <c r="D116">
+        <v>60104</v>
+      </c>
+      <c r="E116">
+        <v>60118</v>
+      </c>
+      <c r="F116" s="10">
+        <v>60050.3</v>
+      </c>
+      <c r="G116" s="10">
+        <v>59765.21</v>
+      </c>
+      <c r="H116" s="10">
+        <v>59831.19</v>
+      </c>
+      <c r="I116" s="10">
+        <v>60422.96</v>
+      </c>
+      <c r="J116" s="10">
+        <v>60986.559999999998</v>
+      </c>
+      <c r="K116" s="10">
+        <v>62187.55</v>
+      </c>
+      <c r="L116" s="10">
+        <v>63088.43</v>
+      </c>
+      <c r="M116" s="10">
+        <v>63510.67</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>309</v>
+      </c>
+      <c r="B117">
+        <v>67531</v>
+      </c>
+      <c r="C117">
+        <v>67206</v>
+      </c>
+      <c r="D117">
+        <v>66829</v>
+      </c>
+      <c r="E117">
+        <v>65628</v>
+      </c>
+      <c r="F117" s="10">
+        <v>62639.75</v>
+      </c>
+      <c r="G117" s="10">
+        <v>62278.02</v>
+      </c>
+      <c r="H117" s="10">
+        <v>63140.17</v>
+      </c>
+      <c r="I117" s="10">
+        <v>64892.77</v>
+      </c>
+      <c r="J117" s="10">
+        <v>66403.429999999993</v>
+      </c>
+      <c r="K117" s="10">
+        <v>69011.399999999994</v>
+      </c>
+      <c r="L117" s="10">
+        <v>70398.179999999993</v>
+      </c>
+      <c r="M117" s="10">
+        <v>70518.13</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>310</v>
+      </c>
+      <c r="B118">
+        <v>78634</v>
+      </c>
+      <c r="C118">
+        <v>81114</v>
+      </c>
+      <c r="D118">
+        <v>82567</v>
+      </c>
+      <c r="E118">
+        <v>81708</v>
+      </c>
+      <c r="F118" s="10">
+        <v>80788.13</v>
+      </c>
+      <c r="G118" s="10">
+        <v>77991.12</v>
+      </c>
+      <c r="H118" s="10">
+        <v>77992.899999999994</v>
+      </c>
+      <c r="I118" s="10">
+        <v>81390.48</v>
+      </c>
+      <c r="J118" s="10">
+        <v>84974.61</v>
+      </c>
+      <c r="K118" s="10">
+        <v>92469.52</v>
+      </c>
+      <c r="L118" s="10">
+        <v>99340.25</v>
+      </c>
+      <c r="M118" s="10">
+        <v>103071.51</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>311</v>
+      </c>
+      <c r="B119">
+        <v>73255</v>
+      </c>
+      <c r="C119">
+        <v>73903</v>
+      </c>
+      <c r="D119">
+        <v>75208</v>
+      </c>
+      <c r="E119">
+        <v>77549</v>
+      </c>
+      <c r="F119" s="10">
+        <v>79472.56</v>
+      </c>
+      <c r="G119" s="10">
+        <v>81022.880000000005</v>
+      </c>
+      <c r="H119" s="10">
+        <v>84088.22</v>
+      </c>
+      <c r="I119" s="10">
+        <v>88162.09</v>
+      </c>
+      <c r="J119" s="10">
+        <v>90915.95</v>
+      </c>
+      <c r="K119" s="10">
+        <v>96999.19</v>
+      </c>
+      <c r="L119" s="10">
+        <v>101726.35</v>
+      </c>
+      <c r="M119" s="10">
+        <v>104455.73</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>312</v>
+      </c>
+      <c r="B120">
+        <v>79087</v>
+      </c>
+      <c r="C120">
+        <v>78692</v>
+      </c>
+      <c r="D120">
+        <v>77433</v>
+      </c>
+      <c r="E120">
+        <v>75962</v>
+      </c>
+      <c r="F120" s="10">
+        <v>74316.800000000003</v>
+      </c>
+      <c r="G120" s="10">
+        <v>73823.039999999994</v>
+      </c>
+      <c r="H120" s="10">
+        <v>74820.899999999994</v>
+      </c>
+      <c r="I120" s="10">
+        <v>76865.11</v>
+      </c>
+      <c r="J120" s="10">
+        <v>79716.17</v>
+      </c>
+      <c r="K120" s="10">
+        <v>83679.570000000007</v>
+      </c>
+      <c r="L120" s="10">
+        <v>88181.31</v>
+      </c>
+      <c r="M120" s="10">
+        <v>92608.46</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>313</v>
+      </c>
+      <c r="B121">
+        <v>76347</v>
+      </c>
+      <c r="C121">
+        <v>75378</v>
+      </c>
+      <c r="D121">
+        <v>75186</v>
+      </c>
+      <c r="E121">
+        <v>75601</v>
+      </c>
+      <c r="F121" s="10">
+        <v>77506.92</v>
+      </c>
+      <c r="G121" s="10">
+        <v>78280.3</v>
+      </c>
+      <c r="H121" s="10">
+        <v>77699.53</v>
+      </c>
+      <c r="I121" s="10">
+        <v>76173.39</v>
+      </c>
+      <c r="J121" s="10">
+        <v>74563.95</v>
+      </c>
+      <c r="K121" s="10">
+        <v>72841.52</v>
+      </c>
+      <c r="L121" s="10">
+        <v>73026.559999999998</v>
+      </c>
+      <c r="M121" s="10">
+        <v>74801.19</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>314</v>
+      </c>
+      <c r="B122">
+        <v>76049</v>
+      </c>
+      <c r="C122">
+        <v>75826</v>
+      </c>
+      <c r="D122">
+        <v>76076</v>
+      </c>
+      <c r="E122">
+        <v>74745</v>
+      </c>
+      <c r="F122" s="10">
+        <v>73736.05</v>
+      </c>
+      <c r="G122" s="10">
+        <v>72955.33</v>
+      </c>
+      <c r="H122" s="10">
+        <v>72205.61</v>
+      </c>
+      <c r="I122" s="10">
+        <v>72001.95</v>
+      </c>
+      <c r="J122" s="10">
+        <v>72987.62</v>
+      </c>
+      <c r="K122" s="10">
+        <v>74502.5</v>
+      </c>
+      <c r="L122" s="10">
+        <v>75047.070000000007</v>
+      </c>
+      <c r="M122" s="10">
+        <v>74691.06</v>
+      </c>
+    </row>
+    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>315</v>
+      </c>
+      <c r="B123">
+        <v>69221</v>
+      </c>
+      <c r="C123">
+        <v>70319</v>
+      </c>
+      <c r="D123">
+        <v>70871</v>
+      </c>
+      <c r="E123">
+        <v>71813</v>
+      </c>
+      <c r="F123" s="10">
+        <v>72374.990000000005</v>
+      </c>
+      <c r="G123" s="10">
+        <v>72914.42</v>
+      </c>
+      <c r="H123" s="10">
+        <v>73133.679999999993</v>
+      </c>
+      <c r="I123" s="10">
+        <v>73140.789999999994</v>
+      </c>
+      <c r="J123" s="10">
+        <v>72572.070000000007</v>
+      </c>
+      <c r="K123" s="10">
+        <v>70928.600000000006</v>
+      </c>
+      <c r="L123" s="10">
+        <v>69411.62</v>
+      </c>
+      <c r="M123" s="10">
+        <v>68346.990000000005</v>
+      </c>
+    </row>
+    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>316</v>
+      </c>
+      <c r="B124">
+        <v>57573</v>
+      </c>
+      <c r="C124">
+        <v>58716</v>
+      </c>
+      <c r="D124">
+        <v>60038</v>
+      </c>
+      <c r="E124">
+        <v>61981</v>
+      </c>
+      <c r="F124" s="10">
+        <v>64027.87</v>
+      </c>
+      <c r="G124" s="10">
+        <v>65818.7</v>
+      </c>
+      <c r="H124" s="10">
+        <v>66939.5</v>
+      </c>
+      <c r="I124" s="10">
+        <v>67629.759999999995</v>
+      </c>
+      <c r="J124" s="10">
+        <v>68290.83</v>
+      </c>
+      <c r="K124" s="10">
+        <v>68370.34</v>
+      </c>
+      <c r="L124" s="10">
+        <v>68258.13</v>
+      </c>
+      <c r="M124" s="10">
+        <v>68227.17</v>
+      </c>
+    </row>
+    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>317</v>
+      </c>
+      <c r="B125">
+        <v>41636</v>
+      </c>
+      <c r="C125">
+        <v>44087</v>
+      </c>
+      <c r="D125">
+        <v>46285</v>
+      </c>
+      <c r="E125">
+        <v>49447</v>
+      </c>
+      <c r="F125" s="10">
+        <v>51988.85</v>
+      </c>
+      <c r="G125" s="10">
+        <v>53059.24</v>
+      </c>
+      <c r="H125" s="10">
+        <v>54307.88</v>
+      </c>
+      <c r="I125" s="10">
+        <v>55333.1</v>
+      </c>
+      <c r="J125" s="10">
+        <v>56680.78</v>
+      </c>
+      <c r="K125" s="10">
+        <v>57429.48</v>
+      </c>
+      <c r="L125" s="10">
+        <v>58253.29</v>
+      </c>
+      <c r="M125" s="10">
+        <v>59084.79</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>318</v>
+      </c>
+      <c r="B126">
+        <v>26770</v>
+      </c>
+      <c r="C126">
+        <v>28588</v>
+      </c>
+      <c r="D126">
+        <v>30352</v>
+      </c>
+      <c r="E126">
+        <v>32165</v>
+      </c>
+      <c r="F126" s="10">
+        <v>33925.129999999997</v>
+      </c>
+      <c r="G126" s="10">
+        <v>37466.06</v>
+      </c>
+      <c r="H126" s="10">
+        <v>39926.68</v>
+      </c>
+      <c r="I126" s="10">
+        <v>41736.080000000002</v>
+      </c>
+      <c r="J126" s="10">
+        <v>43697.14</v>
+      </c>
+      <c r="K126" s="10">
+        <v>45055.59</v>
+      </c>
+      <c r="L126" s="10">
+        <v>44963.78</v>
+      </c>
+      <c r="M126" s="10">
+        <v>45719.76</v>
+      </c>
+    </row>
+    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>319</v>
+      </c>
+      <c r="B127">
+        <v>19048</v>
+      </c>
+      <c r="C127">
+        <v>19637</v>
+      </c>
+      <c r="D127">
+        <v>20346</v>
+      </c>
+      <c r="E127">
+        <v>20930</v>
+      </c>
+      <c r="F127" s="10">
+        <v>21790.44</v>
+      </c>
+      <c r="G127" s="10">
+        <v>23326.26</v>
+      </c>
+      <c r="H127" s="10">
+        <v>25166.560000000001</v>
+      </c>
+      <c r="I127" s="10">
+        <v>26667.45</v>
+      </c>
+      <c r="J127" s="10">
+        <v>28014.16</v>
+      </c>
+      <c r="K127" s="10">
+        <v>28559.38</v>
+      </c>
+      <c r="L127" s="10">
+        <v>30666.07</v>
+      </c>
+      <c r="M127" s="10">
+        <v>32355.67</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>320</v>
+      </c>
+      <c r="B128">
+        <v>15550</v>
+      </c>
+      <c r="C128">
+        <v>15451</v>
+      </c>
+      <c r="D128">
+        <v>15356</v>
+      </c>
+      <c r="E128">
+        <v>15485</v>
+      </c>
+      <c r="F128" s="10">
+        <v>15670.45</v>
+      </c>
+      <c r="G128" s="10">
+        <v>16032.8</v>
+      </c>
+      <c r="H128" s="10">
+        <v>16546.32</v>
+      </c>
+      <c r="I128" s="10">
+        <v>17098.57</v>
+      </c>
+      <c r="J128" s="10">
+        <v>17691.09</v>
+      </c>
+      <c r="K128" s="10">
+        <v>18247.490000000002</v>
+      </c>
+      <c r="L128" s="10">
+        <v>19023.23</v>
+      </c>
+      <c r="M128" s="10">
+        <v>20226.830000000002</v>
+      </c>
+    </row>
+    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>321</v>
+      </c>
+      <c r="B129">
+        <v>11337</v>
+      </c>
+      <c r="C129">
+        <v>11337</v>
+      </c>
+      <c r="D129">
+        <v>11304</v>
+      </c>
+      <c r="E129">
+        <v>11429</v>
+      </c>
+      <c r="F129" s="10">
+        <v>11567.7</v>
+      </c>
+      <c r="G129" s="10">
+        <v>11741.62</v>
+      </c>
+      <c r="H129" s="10">
+        <v>11761.39</v>
+      </c>
+      <c r="I129" s="10">
+        <v>11710.62</v>
+      </c>
+      <c r="J129" s="10">
+        <v>11739.91</v>
+      </c>
+      <c r="K129" s="10">
+        <v>11674.77</v>
+      </c>
+      <c r="L129" s="10">
+        <v>11760.87</v>
+      </c>
+      <c r="M129" s="10">
+        <v>12045.24</v>
+      </c>
+    </row>
+    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>322</v>
+      </c>
+      <c r="B130">
+        <v>10065</v>
+      </c>
+      <c r="C130">
+        <v>10389</v>
+      </c>
+      <c r="D130">
+        <v>10790</v>
+      </c>
+      <c r="E130">
+        <v>11182</v>
+      </c>
+      <c r="F130" s="10">
+        <v>11391.33</v>
+      </c>
+      <c r="G130" s="10">
+        <v>11428.74</v>
+      </c>
+      <c r="H130" s="10">
+        <v>11443.44</v>
+      </c>
+      <c r="I130" s="10">
+        <v>11399.87</v>
+      </c>
+      <c r="J130" s="10">
+        <v>11350.08</v>
+      </c>
+      <c r="K130" s="10">
+        <v>11258.11</v>
+      </c>
+      <c r="L130" s="10">
+        <v>10995.47</v>
+      </c>
+      <c r="M130" s="10">
+        <v>10760.8</v>
+      </c>
+    </row>
+    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>323</v>
+      </c>
+      <c r="B131">
+        <f>SUM(B116:B130)</f>
+        <v>761886</v>
+      </c>
+      <c r="C131">
+        <f t="shared" ref="C131:M131" si="1">SUM(C116:C130)</f>
+        <v>770883</v>
+      </c>
+      <c r="D131">
+        <f t="shared" si="1"/>
+        <v>778745</v>
+      </c>
+      <c r="E131">
+        <f t="shared" si="1"/>
+        <v>785743</v>
+      </c>
+      <c r="F131" s="10">
+        <f t="shared" si="1"/>
+        <v>791247.26999999979</v>
+      </c>
+      <c r="G131" s="10">
+        <f t="shared" si="1"/>
+        <v>797903.73999999987</v>
+      </c>
+      <c r="H131">
+        <f t="shared" si="1"/>
+        <v>809003.97</v>
+      </c>
+      <c r="I131">
+        <f t="shared" si="1"/>
+        <v>824624.98999999987</v>
+      </c>
+      <c r="J131" s="10">
+        <f t="shared" si="1"/>
+        <v>840584.35000000009</v>
+      </c>
+      <c r="K131">
+        <f t="shared" si="1"/>
+        <v>863215.00999999989</v>
+      </c>
+      <c r="L131" s="10">
+        <f t="shared" si="1"/>
+        <v>884140.60999999987</v>
+      </c>
+      <c r="M131">
+        <f t="shared" si="1"/>
+        <v>900424.00000000012</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
revised duration of infection
</commit_message>
<xml_diff>
--- a/GC_HIV_ModelParameters.xlsx
+++ b/GC_HIV_ModelParameters.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\AAPS_model\AAPPS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\AAPS_model\AAPPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17895" windowHeight="8970" tabRatio="682" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17505" windowHeight="7080" tabRatio="682" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="References" sheetId="12" r:id="rId1"/>
@@ -935,7 +935,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="171" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -1606,7 +1606,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
@@ -2605,6 +2605,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="554243408"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -5465,8 +5466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:V94"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5878,16 +5879,16 @@
       <c r="B19" s="3">
         <v>0.1</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="1">
         <v>0.1</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="1">
         <v>0.1</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="1">
         <v>0.1</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19" s="1">
         <v>0.1</v>
       </c>
       <c r="G19" t="s">
@@ -6196,19 +6197,19 @@
         <v>66</v>
       </c>
       <c r="B33">
-        <v>75</v>
+        <v>346</v>
       </c>
       <c r="C33">
-        <v>75</v>
+        <v>346</v>
       </c>
       <c r="D33">
-        <v>75</v>
+        <v>346</v>
       </c>
       <c r="E33">
-        <v>75</v>
+        <v>346</v>
       </c>
       <c r="F33">
-        <v>75</v>
+        <v>346</v>
       </c>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
@@ -6218,19 +6219,19 @@
         <v>67</v>
       </c>
       <c r="B34">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="C34">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="D34">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="E34">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="F34">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="G34" s="3" t="s">
         <v>171</v>
@@ -6263,19 +6264,19 @@
         <v>68</v>
       </c>
       <c r="B35">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="C35">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D35">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E35">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="F35">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="O35">
         <f t="shared" si="0"/>
@@ -7062,7 +7063,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+    <sheetView topLeftCell="A100" workbookViewId="0">
       <selection activeCell="D123" sqref="D123"/>
     </sheetView>
   </sheetViews>
@@ -7576,7 +7577,7 @@
         <v>4914</v>
       </c>
       <c r="E102" s="82">
-        <f>D102/F102*100</f>
+        <f t="shared" ref="E102:E110" si="0">D102/F102*100</f>
         <v>11.183347708509524</v>
       </c>
       <c r="F102" s="10">
@@ -7599,7 +7600,7 @@
         <v>5080</v>
       </c>
       <c r="E103" s="82">
-        <f>D103/F103*100</f>
+        <f t="shared" si="0"/>
         <v>11.444414669441711</v>
       </c>
       <c r="F103" s="10">
@@ -7622,7 +7623,7 @@
         <v>5230</v>
       </c>
       <c r="E104" s="82">
-        <f>D104/F104*100</f>
+        <f t="shared" si="0"/>
         <v>11.677404184944985</v>
       </c>
       <c r="F104" s="10">
@@ -7645,7 +7646,7 @@
         <v>5384</v>
       </c>
       <c r="E105" s="82">
-        <f>D105/F105*100</f>
+        <f t="shared" si="0"/>
         <v>11.937626066106644</v>
       </c>
       <c r="F105" s="10">
@@ -7669,7 +7670,7 @@
         <v>5516</v>
       </c>
       <c r="E106" s="82">
-        <f>D106/F106*100</f>
+        <f t="shared" si="0"/>
         <v>12.1282712404082</v>
       </c>
       <c r="F106" s="10">
@@ -7705,7 +7706,7 @@
         <v>5828</v>
       </c>
       <c r="E107" s="82">
-        <f>D107/F107*100</f>
+        <f t="shared" si="0"/>
         <v>12.638456401528872</v>
       </c>
       <c r="F107" s="10">
@@ -7741,7 +7742,7 @@
         <v>5275</v>
       </c>
       <c r="E108" s="82">
-        <f>D108/F108*100</f>
+        <f t="shared" si="0"/>
         <v>10.317495369778975</v>
       </c>
       <c r="F108" s="10">
@@ -7777,7 +7778,7 @@
         <v>5341</v>
       </c>
       <c r="E109" s="82">
-        <f>D109/F109*100</f>
+        <f t="shared" si="0"/>
         <v>10.085576513264584</v>
       </c>
       <c r="F109" s="10">
@@ -7813,7 +7814,7 @@
         <v>5199</v>
       </c>
       <c r="E110" s="82">
-        <f>D110/F110*100</f>
+        <f t="shared" si="0"/>
         <v>9.4106768370489764</v>
       </c>
       <c r="F110" s="10">
@@ -8551,47 +8552,47 @@
         <v>761886</v>
       </c>
       <c r="C132">
-        <f t="shared" ref="C132:M132" si="0">SUM(C117:C131)</f>
+        <f t="shared" ref="C132:M132" si="1">SUM(C117:C131)</f>
         <v>770883</v>
       </c>
       <c r="D132">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>778745</v>
       </c>
       <c r="E132">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>785743</v>
       </c>
       <c r="F132" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>791247.26999999979</v>
       </c>
       <c r="G132" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>797903.73999999987</v>
       </c>
       <c r="H132">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>809003.97</v>
       </c>
       <c r="I132">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>824624.98999999987</v>
       </c>
       <c r="J132" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>840584.35000000009</v>
       </c>
       <c r="K132">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>863215.00999999989</v>
       </c>
       <c r="L132" s="10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>884140.60999999987</v>
       </c>
       <c r="M132">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>900424.00000000012</v>
       </c>
     </row>
@@ -8637,14 +8638,14 @@
         <v>375</v>
       </c>
       <c r="C137" s="86">
-        <f>B137/F106*100</f>
+        <f t="shared" ref="C137:C142" si="2">B137/F106*100</f>
         <v>0.82452895488634415</v>
       </c>
       <c r="D137">
         <v>362</v>
       </c>
       <c r="E137" s="86">
-        <f>D137/F106*100</f>
+        <f t="shared" ref="E137:E142" si="3">D137/F106*100</f>
         <v>0.79594528445028434</v>
       </c>
       <c r="F137">
@@ -8670,28 +8671,28 @@
         <v>429</v>
       </c>
       <c r="C138" s="86">
-        <f>B138/F107*100</f>
+        <f t="shared" si="2"/>
         <v>0.93031877080574576</v>
       </c>
       <c r="D138">
         <v>363</v>
       </c>
       <c r="E138" s="86">
-        <f>D138/F107*100</f>
+        <f t="shared" si="3"/>
         <v>0.78719280606640041</v>
       </c>
       <c r="F138">
         <v>521</v>
       </c>
       <c r="G138" s="86">
-        <f t="shared" ref="G138:G142" si="1">F138/F107*100</f>
+        <f t="shared" ref="G138:G142" si="4">F138/F107*100</f>
         <v>1.1298276913515002</v>
       </c>
       <c r="H138">
         <v>1045</v>
       </c>
       <c r="I138" s="86">
-        <f t="shared" ref="I138:I142" si="2">H138/F107*100</f>
+        <f t="shared" ref="I138:I142" si="5">H138/F107*100</f>
         <v>2.2661611083729705</v>
       </c>
     </row>
@@ -8703,28 +8704,28 @@
         <v>485</v>
       </c>
       <c r="C139" s="86">
-        <f>B139/F108*100</f>
+        <f t="shared" si="2"/>
         <v>0.94862279703181085</v>
       </c>
       <c r="D139">
         <v>432</v>
       </c>
       <c r="E139" s="86">
-        <f>D139/F108*100</f>
+        <f t="shared" si="3"/>
         <v>0.84495886251080898</v>
       </c>
       <c r="F139">
         <v>544</v>
       </c>
       <c r="G139" s="86">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1.0640222713099077</v>
       </c>
       <c r="H139">
         <v>1174</v>
       </c>
       <c r="I139" s="86">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>2.2962539458048372</v>
       </c>
     </row>
@@ -8736,28 +8737,28 @@
         <v>662</v>
       </c>
       <c r="C140" s="86">
-        <f>B140/F109*100</f>
+        <f t="shared" si="2"/>
         <v>1.250075201606657</v>
       </c>
       <c r="D140" s="10">
         <v>513</v>
       </c>
       <c r="E140" s="86">
-        <f>D140/F109*100</f>
+        <f t="shared" si="3"/>
         <v>0.96871386468914655</v>
       </c>
       <c r="F140">
         <v>623</v>
       </c>
       <c r="G140" s="86">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1.1764302879168387</v>
       </c>
       <c r="H140">
         <v>1456</v>
       </c>
       <c r="I140" s="86">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>2.7494101110865445</v>
       </c>
     </row>
@@ -8769,28 +8770,28 @@
         <v>809</v>
       </c>
       <c r="C141" s="86">
-        <f>B141/F110*100</f>
+        <f t="shared" si="2"/>
         <v>1.4643657551784233</v>
       </c>
       <c r="D141">
         <v>608</v>
       </c>
       <c r="E141" s="86">
-        <f>D141/F110*100</f>
+        <f t="shared" si="3"/>
         <v>1.1005369334344639</v>
       </c>
       <c r="F141">
         <v>854</v>
       </c>
       <c r="G141" s="86">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1.5458199690016976</v>
       </c>
       <c r="H141">
         <v>1821</v>
       </c>
       <c r="I141" s="86">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>3.2961805193818403</v>
       </c>
     </row>
@@ -8802,28 +8803,28 @@
         <v>1061</v>
       </c>
       <c r="C142" s="86">
-        <f>B142/F111*100</f>
+        <f t="shared" si="2"/>
         <v>1.8182354021446405</v>
       </c>
       <c r="D142">
         <v>743</v>
       </c>
       <c r="E142" s="86">
-        <f>D142/F111*100</f>
+        <f t="shared" si="3"/>
         <v>1.2732788914170292</v>
       </c>
       <c r="F142">
         <v>1119</v>
       </c>
       <c r="G142" s="86">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1.9176299858622552</v>
       </c>
       <c r="H142">
         <v>2284</v>
       </c>
       <c r="I142" s="86">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>3.9140901588108941</v>
       </c>
     </row>

</xml_diff>